<commit_message>
to make the second curve
</commit_message>
<xml_diff>
--- a/work_function/datasheet.xlsx
+++ b/work_function/datasheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Phy_op\work_function\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A052CAE-68DF-4D31-A771-E6ECDEE8EB5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCD999F-8901-4BE2-9E3D-370F82B033E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -243,6 +243,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -267,86 +273,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1592,10 +1524,6 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN"/>
-              <a:t>lg(I_e/T^2)~1/T</a:t>
-            </a:r>
-            <a:r>
               <a:rPr lang="zh-CN" altLang="en-US"/>
               <a:t>曲线</a:t>
             </a:r>
@@ -1633,7 +1561,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.7452318880670769E-2"/>
+          <c:y val="0.12729436029185898"/>
+          <c:w val="0.76080801532725495"/>
+          <c:h val="0.68588058355839776"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -3070,15 +3008,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>71802</xdr:colOff>
+      <xdr:colOff>71801</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>17957</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>529002</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>184980</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>563216</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>79513</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3684,8 +3622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -3726,25 +3664,25 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="7">
         <v>6</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="7">
         <v>7</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="7">
         <v>8</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="7">
         <v>9</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="7">
         <v>10</v>
       </c>
-      <c r="G3" s="15">
+      <c r="G3" s="7">
         <v>11</v>
       </c>
-      <c r="H3" s="15">
+      <c r="H3" s="7">
         <v>12</v>
       </c>
       <c r="J3" t="s">
@@ -3776,31 +3714,31 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="7">
         <f t="shared" ref="B4:H9" si="0">LOG10(M2)-3</f>
         <v>-2.4881166390211256</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="7">
         <f t="shared" si="0"/>
         <v>-2.4801720062242811</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="7">
         <f t="shared" si="0"/>
         <v>-2.4710832997223453</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="7">
         <f t="shared" si="0"/>
         <v>-2.4621809049267256</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="7">
         <f t="shared" si="0"/>
         <v>-2.4534573365218688</v>
       </c>
-      <c r="G4" s="15">
+      <c r="G4" s="7">
         <f t="shared" si="0"/>
         <v>-2.4449055514216811</v>
       </c>
-      <c r="H4" s="15">
+      <c r="H4" s="7">
         <f t="shared" si="0"/>
         <v>-2.4353339357479107</v>
       </c>
@@ -3833,31 +3771,31 @@
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="7">
         <f t="shared" si="0"/>
         <v>-2.0438315695246367</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="7">
         <f t="shared" si="0"/>
         <v>-2.034798298974088</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="7">
         <f t="shared" si="0"/>
         <v>-2.0268721464003012</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="7">
         <f t="shared" si="0"/>
         <v>-2.0177287669604316</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="7">
         <f t="shared" si="0"/>
         <v>-2.0096611452123985</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="7">
         <f t="shared" si="0"/>
         <v>-2.000869458712629</v>
       </c>
-      <c r="H5" s="15">
+      <c r="H5" s="7">
         <f t="shared" si="0"/>
         <v>-1.9909742579130898</v>
       </c>
@@ -3890,31 +3828,31 @@
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="7">
         <f t="shared" si="0"/>
         <v>-1.6259852597080884</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="7">
         <f t="shared" si="0"/>
         <v>-1.6178027896225464</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="7">
         <f t="shared" si="0"/>
         <v>-1.6092414712612828</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="7">
         <f t="shared" si="0"/>
         <v>-1.6024075659618833</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="7">
         <f t="shared" si="0"/>
         <v>-1.5951662833800619</v>
       </c>
-      <c r="G6" s="15">
+      <c r="G6" s="7">
         <f t="shared" si="0"/>
         <v>-1.5855280503706972</v>
       </c>
-      <c r="H6" s="15">
+      <c r="H6" s="7">
         <f t="shared" si="0"/>
         <v>-1.5774101601485178</v>
       </c>
@@ -3947,31 +3885,31 @@
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="7">
         <f t="shared" si="0"/>
         <v>-1.2974833025618495</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="7">
         <f t="shared" si="0"/>
         <v>-1.290051983489239</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="7">
         <f t="shared" si="0"/>
         <v>-1.2824127031445396</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="7">
         <f t="shared" si="0"/>
         <v>-1.2748236985808628</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="7">
         <f t="shared" si="0"/>
         <v>-1.2677671197795022</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="7">
         <f t="shared" si="0"/>
         <v>-1.2597952644925503</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="7">
         <f t="shared" si="0"/>
         <v>-1.2509597312965428</v>
       </c>
@@ -4004,31 +3942,31 @@
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="7">
         <f t="shared" si="0"/>
         <v>-0.96345094552084776</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="7">
         <f t="shared" si="0"/>
         <v>-0.95577392288731744</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="7">
         <f t="shared" si="0"/>
         <v>-0.94842304152746015</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="7">
         <f t="shared" si="0"/>
         <v>-0.94055018749203922</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="7">
         <f t="shared" si="0"/>
         <v>-0.9337486380310378</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8" s="7">
         <f t="shared" si="0"/>
         <v>-0.92617171559889133</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="7">
         <f t="shared" si="0"/>
         <v>-0.91847267375519515</v>
       </c>
@@ -4040,31 +3978,31 @@
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="7">
         <f t="shared" si="0"/>
         <v>-0.6599526823386066</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="7">
         <f t="shared" si="0"/>
         <v>-0.6520848134983086</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="7">
         <f t="shared" si="0"/>
         <v>-0.64493179365114939</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="7">
         <f t="shared" si="0"/>
         <v>-0.63770606203576907</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="7">
         <f t="shared" si="0"/>
         <v>-0.63096977819084676</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="7">
         <f t="shared" si="0"/>
         <v>-0.62305824285324141</v>
       </c>
-      <c r="H9" s="15">
+      <c r="H9" s="7">
         <f t="shared" si="0"/>
         <v>-0.61546738450575145</v>
       </c>
@@ -4161,7 +4099,7 @@
     </row>
     <row r="18" spans="1:19" ht="44.4" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S19" s="14"/>
+      <c r="S19" s="6"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -4239,50 +4177,50 @@
     </row>
     <row r="35" spans="12:28" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="36" spans="12:28" x14ac:dyDescent="0.25">
-      <c r="T36" s="8" t="s">
+      <c r="T36" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="U36" s="10"/>
-      <c r="V36" s="12"/>
-      <c r="W36" s="6"/>
-      <c r="X36" s="6"/>
-      <c r="Y36" s="6"/>
-      <c r="Z36" s="6"/>
-      <c r="AA36" s="6"/>
-      <c r="AB36" s="6"/>
+      <c r="U36" s="12"/>
+      <c r="V36" s="14"/>
+      <c r="W36" s="8"/>
+      <c r="X36" s="8"/>
+      <c r="Y36" s="8"/>
+      <c r="Z36" s="8"/>
+      <c r="AA36" s="8"/>
+      <c r="AB36" s="8"/>
     </row>
     <row r="37" spans="12:28" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="T37" s="9"/>
-      <c r="U37" s="11"/>
-      <c r="V37" s="13"/>
-      <c r="W37" s="7"/>
-      <c r="X37" s="7"/>
-      <c r="Y37" s="7"/>
-      <c r="Z37" s="7"/>
-      <c r="AA37" s="7"/>
-      <c r="AB37" s="7"/>
+      <c r="T37" s="11"/>
+      <c r="U37" s="13"/>
+      <c r="V37" s="15"/>
+      <c r="W37" s="9"/>
+      <c r="X37" s="9"/>
+      <c r="Y37" s="9"/>
+      <c r="Z37" s="9"/>
+      <c r="AA37" s="9"/>
+      <c r="AB37" s="9"/>
     </row>
     <row r="38" spans="12:28" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L38" s="15">
+      <c r="L38" s="7">
         <v>1726</v>
       </c>
-      <c r="M38" s="15">
+      <c r="M38" s="7">
         <f>1726+0.6*(1809-1726)</f>
         <v>1775.8</v>
       </c>
-      <c r="N38" s="15">
+      <c r="N38" s="7">
         <f>1809+0.2*(1901-1809)</f>
         <v>1827.4</v>
       </c>
-      <c r="O38" s="15">
+      <c r="O38" s="7">
         <f>1901-0.2*(1901-1809)</f>
         <v>1882.6</v>
       </c>
-      <c r="P38" s="15">
+      <c r="P38" s="7">
         <f>1901+0.4*(1975-1901)</f>
         <v>1930.6</v>
       </c>
-      <c r="Q38" s="15">
+      <c r="Q38" s="7">
         <v>1975</v>
       </c>
       <c r="T38" s="3">
@@ -4312,27 +4250,27 @@
       </c>
     </row>
     <row r="39" spans="12:28" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L39" s="15">
+      <c r="L39" s="7">
         <f t="shared" ref="L39:Q39" si="3">-1/L38</f>
         <v>-5.7937427578215526E-4</v>
       </c>
-      <c r="M39" s="15">
+      <c r="M39" s="7">
         <f t="shared" si="3"/>
         <v>-5.631264782070053E-4</v>
       </c>
-      <c r="N39" s="15">
+      <c r="N39" s="7">
         <f t="shared" si="3"/>
         <v>-5.472255663784612E-4</v>
       </c>
-      <c r="O39" s="15">
+      <c r="O39" s="7">
         <f t="shared" si="3"/>
         <v>-5.3118028258791034E-4</v>
       </c>
-      <c r="P39" s="15">
+      <c r="P39" s="7">
         <f t="shared" si="3"/>
         <v>-5.1797368693670361E-4</v>
       </c>
-      <c r="Q39" s="15">
+      <c r="Q39" s="7">
         <f t="shared" si="3"/>
         <v>-5.0632911392405066E-4</v>
       </c>
@@ -4363,22 +4301,22 @@
       </c>
     </row>
     <row r="40" spans="12:28" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L40" s="15">
+      <c r="L40" s="7">
         <v>-2.5414129120704159</v>
       </c>
-      <c r="M40" s="15">
+      <c r="M40" s="7">
         <v>-2.0961324329892657</v>
       </c>
-      <c r="N40" s="15">
+      <c r="N40" s="7">
         <v>-1.6740470002637498</v>
       </c>
-      <c r="O40" s="15">
+      <c r="O40" s="7">
         <v>-1.3437765296346198</v>
       </c>
-      <c r="P40" s="15">
+      <c r="P40" s="7">
         <v>-1.0080602571279731</v>
       </c>
-      <c r="Q40" s="15">
+      <c r="Q40" s="7">
         <v>-0.70378294573341837</v>
       </c>
       <c r="T40" s="3">
@@ -4408,22 +4346,22 @@
       </c>
     </row>
     <row r="41" spans="12:28" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L41" s="15">
+      <c r="L41" s="7">
         <v>0.99984116842064097</v>
       </c>
-      <c r="M41" s="15">
+      <c r="M41" s="7">
         <v>0.99967730582369929</v>
       </c>
-      <c r="N41" s="15">
+      <c r="N41" s="7">
         <v>0.99925621325203196</v>
       </c>
-      <c r="O41" s="15">
+      <c r="O41" s="7">
         <v>0.99960170454529118</v>
       </c>
-      <c r="P41" s="15">
+      <c r="P41" s="7">
         <v>0.99991021445392647</v>
       </c>
-      <c r="Q41" s="15">
+      <c r="Q41" s="7">
         <v>0.99981403215932763</v>
       </c>
       <c r="T41" s="3">

</xml_diff>